<commit_message>
fixed problems with networks
</commit_message>
<xml_diff>
--- a/grid_search.xlsx
+++ b/grid_search.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Desktop\Alessio-Work\Repositories\bioformer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7A49B44-203D-4755-8159-545F0C40A35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="81480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,55 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>tcn_layers</t>
+  </si>
+  <si>
+    <t>blocks</t>
+  </si>
+  <si>
+    <t>dim_head</t>
+  </si>
+  <si>
+    <t>heads</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>patch1</t>
+  </si>
+  <si>
+    <t>patch2</t>
+  </si>
+  <si>
+    <t>patch3</t>
+  </si>
+  <si>
+    <t>ch1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch2 </t>
+  </si>
+  <si>
+    <t>ch3</t>
+  </si>
+  <si>
+    <t>ViT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +383,411 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="A2:I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.86328125" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
+      <c r="L3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>14</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="M7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="K9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added adaptive on input features
</commit_message>
<xml_diff>
--- a/grid_search.xlsx
+++ b/grid_search.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Desktop\Alessio-Work\Repositories\bioformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F006681-8051-4187-9645-1176F76360FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1327953E-0853-4AE3-9116-9DD07371F78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="81480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,11 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -419,7 +418,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="M9" sqref="C9:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -472,130 +471,105 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
-        <v>32</v>
-      </c>
-      <c r="F3" s="3">
-        <v>8</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3">
-        <v>14</v>
-      </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
-        <v>32</v>
-      </c>
-      <c r="F4" s="3">
-        <v>8</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>5</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3">
-        <v>14</v>
-      </c>
-      <c r="L4" s="3">
+      <c r="K4">
+        <v>14</v>
+      </c>
+      <c r="L4">
         <v>16</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" s="3">
-        <v>32</v>
-      </c>
-      <c r="F5" s="3">
-        <v>8</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
+      <c r="E5">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="K5" s="3">
-        <v>14</v>
-      </c>
-      <c r="L5" s="3">
+      <c r="K5">
+        <v>14</v>
+      </c>
+      <c r="L5">
         <v>16</v>
       </c>
-      <c r="M5" s="3">
-        <v>32</v>
-      </c>
-      <c r="N5" s="3"/>
+      <c r="M5">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
@@ -627,83 +601,76 @@
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="E7" s="3">
-        <v>32</v>
-      </c>
-      <c r="F7" s="3">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>3</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3">
-        <v>14</v>
-      </c>
-      <c r="L7" s="3">
+      <c r="K7">
+        <v>14</v>
+      </c>
+      <c r="L7">
         <v>16</v>
       </c>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" s="3">
-        <v>32</v>
-      </c>
-      <c r="F8" s="3">
-        <v>8</v>
-      </c>
-      <c r="G8" s="3">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
+      <c r="E8">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>5</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <v>3</v>
       </c>
-      <c r="K8" s="3">
-        <v>14</v>
-      </c>
-      <c r="L8" s="3">
+      <c r="K8">
+        <v>14</v>
+      </c>
+      <c r="L8">
         <v>16</v>
       </c>
-      <c r="M8" s="3">
-        <v>32</v>
-      </c>
-      <c r="N8" s="3"/>
+      <c r="M8">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
@@ -735,39 +702,32 @@
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
-        <v>32</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>32</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="G10" s="3">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3">
-        <v>10</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3">
-        <v>14</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
@@ -799,71 +759,58 @@
       </c>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>16</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>4</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="H12" s="3">
-        <v>10</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3">
-        <v>14</v>
-      </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3">
-        <v>32</v>
-      </c>
-      <c r="F13" s="3">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>32</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13">
         <v>2</v>
       </c>
-      <c r="H13" s="3">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3">
-        <v>14</v>
-      </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>14</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>

</xml_diff>